<commit_message>
Improved domain adaption and handling of wall boundary conditions
</commit_message>
<xml_diff>
--- a/AttributeVocabulary.xlsx
+++ b/AttributeVocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skarman/Pointwise/omega/consulting/MIT_AutoMesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F76811-B094-474D-B8E2-6E34BFB35D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37065F3F-89B2-5F4E-97B2-528DEADD49E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24060" yWindow="11200" windowWidth="23600" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,8 +788,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,7 +1404,7 @@
         <v>99</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Various updates for periodic entities and baffles
Added support for periodic connectors and domains during export of mesh associativity (including a new version of mesh associativity file format).  Updated examples. Added some new meshing parameters. Removed QuiltToSurfMesh script (automated volume meshing only). Better handling of wake sheets (baffles).
</commit_message>
<xml_diff>
--- a/AttributeVocabulary.xlsx
+++ b/AttributeVocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skarman/Pointwise/omega/consulting/MIT_AutoMesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37065F3F-89B2-5F4E-97B2-528DEADD49E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DE98231-7B08-8244-9C2D-4CE3E10C1B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="11200" windowWidth="23600" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22840" yWindow="7100" windowWidth="23600" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeomToMesh Attributes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="114">
   <si>
     <t>Key</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>Set the domain shape constraint</t>
+  </si>
+  <si>
+    <t>PW:DomainBlunt</t>
+  </si>
+  <si>
+    <t>Flag the domain as blunt for special dimension handling</t>
   </si>
 </sst>
 </file>
@@ -788,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,10 +1161,18 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -1174,7 +1188,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>

</xml_diff>